<commit_message>
Printing outputs for final paper
</commit_message>
<xml_diff>
--- a/data/r16_augie.xlsx
+++ b/data/r16_augie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/augustusge/Desktop/Brown Biostats/PHP2550/Final/predicting-wimbledon-matches/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71D50EEF-8780-5C4B-9FD7-763A081EBD24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{565231D3-3956-7744-BCA1-B91344241DA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{3829C63B-7C12-7443-B6E1-E5A3B0556EEA}"/>
   </bookViews>
@@ -99,13 +99,13 @@
     <t>Berrettini M.</t>
   </si>
   <si>
-    <t>Quarter</t>
-  </si>
-  <si>
-    <t>Semis</t>
+    <t>Quarterfinals</t>
   </si>
   <si>
     <t>Finals</t>
+  </si>
+  <si>
+    <t>Semifinals</t>
   </si>
 </sst>
 </file>
@@ -460,7 +460,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20:E21"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -629,10 +629,10 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E10">
-        <v>37</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -688,7 +688,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
@@ -705,7 +705,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
         <v>16</v>
@@ -722,7 +722,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>

</xml_diff>